<commit_message>
added methods to the lecturer model class and tried a first unit test
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29058006-22D3-4F15-B52A-52DBE5EE7E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CC920-D650-4D65-9959-55522C64F1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11400" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -387,6 +387,9 @@
   <si>
     <t>seed data, repositories</t>
   </si>
+  <si>
+    <t>models, 1st test</t>
+  </si>
 </sst>
 </file>
 
@@ -396,7 +399,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yy"/>
     <numFmt numFmtId="165" formatCode="dd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="170" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -892,7 +895,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1024,6 +1027,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC65911"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="7"/>
       </font>
     </dxf>
@@ -1073,11 +1081,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC65911"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2153,7 +2156,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5" s="74">
         <f ca="1">TODAY()</f>
@@ -2202,11 +2205,11 @@
         <v>0.65625</v>
       </c>
       <c r="D5" s="75">
-        <v>0.70486111111111116</v>
+        <v>0.8125</v>
       </c>
       <c r="E5" s="75">
         <f>D5-C5</f>
-        <v>4.861111111111116E-2</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -12278,35 +12281,35 @@
     <row r="23" spans="1:148" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="I24:EP1048576 AD23:EP23 J18:EP22 I6:EP6 I5:ER5 I7:ER17 I3:EP4 I2:AD2 AH2:EP2">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:EH22 I8:ER17">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>High</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:EN6">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"m"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D17">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12948,7 +12951,7 @@
   </sheetData>
   <autoFilter ref="E5:E22" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I18">
-      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="21"/>
+      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="14"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E4:E15">

</xml_diff>

<commit_message>
added PlanaEntity abstract class, added field lessons in lecturersmodules entity class
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2CC920-D650-4D65-9959-55522C64F1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4283D5F-A013-4CF0-B5FA-6813454B9D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11400" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -390,18 +390,288 @@
   <si>
     <t>models, 1st test</t>
   </si>
+  <si>
+    <t>Ablauf der Bachelor-Thesis / Milestones</t>
+  </si>
+  <si>
+    <t>Semester-Woche</t>
+  </si>
+  <si>
+    <t>1  -- 2</t>
+  </si>
+  <si>
+    <t>1 -- 16</t>
+  </si>
+  <si>
+    <t>Ausstellung</t>
+  </si>
+  <si>
+    <t>Prüfungswochen</t>
+  </si>
+  <si>
+    <t>Start Bachelor-Thesis Montag 08h00</t>
+  </si>
+  <si>
+    <t>Festlegen des Deliverables und deren Termine</t>
+  </si>
+  <si>
+    <t>Regelmässige Treffen</t>
+  </si>
+  <si>
+    <t>Abgabe Kurz-Film</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>vormittag</t>
+  </si>
+  <si>
+    <t>14h00-18h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finaltag </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ende Woche 17, </t>
+  </si>
+  <si>
+    <t>20h00</t>
+  </si>
+  <si>
+    <t>10.2.21) mit Experten und Studierenden und melden den Termin an</t>
+  </si>
+  <si>
+    <t>ARB1</t>
+  </si>
+  <si>
+    <t>till 1.12.20</t>
+  </si>
+  <si>
+    <t>ca Oct/Nov</t>
+  </si>
+  <si>
+    <t>wird direkt durch das Sekretariat</t>
+  </si>
+  <si>
+    <t>(Silvia.Gasenzer@bfh.ch)</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <r>
+      <t>Abgabe Texte/Graphiken/etc. für das “</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Book</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>”</t>
+    </r>
+  </si>
+  <si>
+    <t>gem. Moodle (Heinz.Kipfer@bfh.ch)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Abgabe elektronische Version des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Posters</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        25.01.21 - 10.02.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; Moodle</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Öffentliche </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ausstellung</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> der Bachelor-Thesis mit Präsenz der Studierenden</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kurzpräsentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> im Rahmen des Finaltages</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Abgabe Projektdokumentation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> an Betreuer/in und Experten/Expertin; zusätzlich ein Exemplar ans Sekretariat (Archivierung). 
+Eine elektronische Version muss z.Hd. der Abteilung abgegeben werden; Informationen dazu folgen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Betreuer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vereinbaren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ort und Zeit der </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prüfung</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (zwischen 25.1. und</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Verteidigung</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mit Betreuer/in und Experte/Expertin</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yy"/>
     <numFmt numFmtId="165" formatCode="dd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="174" formatCode="ddd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +780,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -751,7 +1029,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -897,6 +1175,17 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="2" xr:uid="{52E8FA25-AB34-439C-BC48-9650F425CC09}"/>
@@ -1027,11 +1316,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FFC65911"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="7"/>
       </font>
     </dxf>
@@ -1081,6 +1365,11 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC65911"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2127,23 +2416,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13538CB-7E67-4044-B4BC-9356A4A96686}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="20.53125" customWidth="1"/>
+    <col min="5" max="5" width="5.53125" style="80" customWidth="1"/>
+    <col min="6" max="6" width="10.265625" style="74" customWidth="1"/>
+    <col min="7" max="7" width="11" style="42" customWidth="1"/>
+    <col min="8" max="8" width="16.46484375" style="77" customWidth="1"/>
+    <col min="9" max="9" width="63" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="str">
         <f>Gannt!A1</f>
         <v>BaThesis BTI7321 20/21, HS, Project Planning</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="72" t="s">
         <v>76</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F3" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="77" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H4" s="68">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H5" s="78" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H6" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="E7" s="80">
+        <f>F7</f>
+        <v>44217</v>
+      </c>
+      <c r="F7" s="74">
+        <v>44217</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="79">
+        <v>16</v>
+      </c>
+      <c r="I7" s="49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H8" s="79"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E9" s="80">
+        <f t="shared" ref="E8:E12" si="0">F9</f>
+        <v>44218</v>
+      </c>
+      <c r="F9" s="74">
+        <v>44218</v>
+      </c>
+      <c r="G9" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E10" s="80">
+        <f t="shared" si="0"/>
+        <v>44218</v>
+      </c>
+      <c r="F10" s="74">
+        <v>44218</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="E11" s="80">
+        <f t="shared" si="0"/>
+        <v>44217</v>
+      </c>
+      <c r="F11" s="74">
+        <v>44217</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F12" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="F16" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="I17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="F19" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>111</v>
+      </c>
+      <c r="J21" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2155,7 +2624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D939E36-8CC7-42CA-89EC-66812AD518D2}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +2668,7 @@
       </c>
       <c r="B5" s="74">
         <f ca="1">TODAY()</f>
-        <v>44061</v>
+        <v>44089</v>
       </c>
       <c r="C5" s="75">
         <v>0.65625</v>
@@ -2466,13 +2935,15 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="9.33203125" customWidth="1"/>
     <col min="3" max="3" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
@@ -2504,6 +2975,9 @@
       </c>
       <c r="D4" s="20" t="s">
         <v>21</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -2780,8 +3254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ER23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3041,11 +3515,11 @@
       <c r="G6" s="58"/>
       <c r="H6" s="58"/>
       <c r="I6" s="48" t="str">
-        <f t="shared" ref="I6:AN6" si="0">LEFT(TEXT(I7,"ddd"),1)</f>
+        <f>LEFT(TEXT(I7,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="48" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I6:AN6" si="0">LEFT(TEXT(J7,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="47" t="str">
@@ -12281,35 +12755,35 @@
     <row r="23" spans="1:148" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="I24:EP1048576 AD23:EP23 J18:EP22 I6:EP6 I5:ER5 I7:ER17 I3:EP4 I2:AD2 AH2:EP2">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:EH22 I8:ER17">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>High</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:EN6">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
       <formula>"m"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D17">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12676,8 +13150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D544E4EA-43A9-4C2D-95F8-E8BC054D1071}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12951,7 +13425,7 @@
   </sheetData>
   <autoFilter ref="E5:E22" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I18">
-      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="14"/>
+      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="21"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E4:E15">

</xml_diff>

<commit_message>
added example of matBlazor page structure
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4283D5F-A013-4CF0-B5FA-6813454B9D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732978D-E161-4D48-9C7C-4B2F47767933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -669,7 +669,7 @@
     <numFmt numFmtId="165" formatCode="dd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
     <numFmt numFmtId="167" formatCode="h:mm;@"/>
-    <numFmt numFmtId="174" formatCode="ddd"/>
+    <numFmt numFmtId="168" formatCode="ddd"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1184,7 +1184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1557,7 +1557,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-In parallel with implementation of api describe it in the main</a:t>
+            <a:t>-In parallel with implementation of api, describe it in the main</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -1594,8 +1594,12 @@
             <a:buChar char="Ø"/>
           </a:pPr>
           <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Project Management document </a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Project Management document with structure for : -PB , - Sprint 1, gannt diagram</a:t>
+            <a:t>with structure for : -PB , - Sprint 1, gannt diagram</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1605,7 +1609,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t> Enter content for PB at the beginning of the sprint</a:t>
+            <a:t> Enter content for the PB at the beginning of the sprint</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1624,8 +1628,8 @@
             <a:buChar char="Ø"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Planner Controller (min -start it)</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>code:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1645,8 +1649,37 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Controllers</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+            <a:buChar char="Ø"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
             <a:t>View -&gt; Planner -&gt;start state</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+            <a:buChar char="Ø"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>report:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> -&gt;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1865,13 +1898,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>  - Start with PlannerController</a:t>
+            <a:t>  </a:t>
           </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
           </a:endParaRPr>
@@ -2418,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13538CB-7E67-4044-B4BC-9356A4A96686}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2507,7 +2535,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E9" s="80">
-        <f t="shared" ref="E8:E12" si="0">F9</f>
+        <f t="shared" ref="E9:E11" si="0">F9</f>
         <v>44218</v>
       </c>
       <c r="F9" s="74">
@@ -2668,7 +2696,7 @@
       </c>
       <c r="B5" s="74">
         <f ca="1">TODAY()</f>
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="C5" s="75">
         <v>0.65625</v>
@@ -3519,7 +3547,7 @@
         <v>M</v>
       </c>
       <c r="J6" s="48" t="str">
-        <f t="shared" ref="I6:AN6" si="0">LEFT(TEXT(J7,"ddd"),1)</f>
+        <f t="shared" ref="J6:AN6" si="0">LEFT(TEXT(J7,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="47" t="str">
@@ -13150,7 +13178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D544E4EA-43A9-4C2D-95F8-E8BC054D1071}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added table with editable cells in for modules view in main plan view
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732978D-E161-4D48-9C7C-4B2F47767933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08435411-CDEA-4325-AB30-EE8EDE170CD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="145">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -174,9 +174,6 @@
     <t xml:space="preserve">User stories </t>
   </si>
   <si>
-    <t>Enter user stories in product backlog</t>
-  </si>
-  <si>
     <t>Break down user stories to tasks for sprint1</t>
   </si>
   <si>
@@ -259,9 +256,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Start first steps of study director's view design with Blazor </t>
-  </si>
-  <si>
     <t>max hs sprint1 = 100h</t>
   </si>
   <si>
@@ -302,23 +296,13 @@
     <t>Management tools</t>
   </si>
   <si>
-    <t>Create project management document structure(PB, sprints,
-gannt diagramm )</t>
-  </si>
-  <si>
     <t xml:space="preserve">max hs sprint1 </t>
   </si>
   <si>
     <t xml:space="preserve"> delivery of sprint1</t>
   </si>
   <si>
-    <t>Make a plan of assignments</t>
-  </si>
-  <si>
     <t>Manage plan of assignments</t>
-  </si>
-  <si>
-    <t>As a study director, I want to be able to make a concrete plan of assignments for lecturers for the coming year as well as a provision plan for the next 2-3 years, so the teachers can be better informed about their work hours and schedule for the next several years. And it will be easier to add new small changes into the employment plan.</t>
   </si>
   <si>
     <t xml:space="preserve">Appointments and Rules </t>
@@ -659,6 +643,97 @@
       <t xml:space="preserve"> mit Betreuer/in und Experte/Expertin</t>
     </r>
   </si>
+  <si>
+    <t>Holidays15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> days-duration
+</t>
+  </si>
+  <si>
+    <t>hours per day</t>
+  </si>
+  <si>
+    <t>As a study director, I want to be able to make a  plan of assignments for lecturers .</t>
+  </si>
+  <si>
+    <t>As a study director, I want to be able to manage a  plan of assignments for lecturers .</t>
+  </si>
+  <si>
+    <t>Make own plan.</t>
+  </si>
+  <si>
+    <t>As a lecturer, I want to be able to manage the plan of my assignments.</t>
+  </si>
+  <si>
+    <t>Manage my plan.</t>
+  </si>
+  <si>
+    <t>As a study director, I want to be able to add groups of lecturers to the module run.</t>
+  </si>
+  <si>
+    <t>Make a group of lecturers.</t>
+  </si>
+  <si>
+    <t>Make a group of modules.</t>
+  </si>
+  <si>
+    <t>As a study director, I want to be able to make a group of module runs.</t>
+  </si>
+  <si>
+    <t>Create a subgroup .</t>
+  </si>
+  <si>
+    <t>As a lecturer, I want to be able to create a subgroup with another lecturer/s.</t>
+  </si>
+  <si>
+    <t>Join a subgroup.</t>
+  </si>
+  <si>
+    <t>As a lecturer, I want to be able to join a subgroup with other lecturer/s.</t>
+  </si>
+  <si>
+    <t>Create a plan of assignments</t>
+  </si>
+  <si>
+    <t>As a lecturer,I want to be able to  add Module Runs in my provision plan.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Ask Mr.Pfahrer if it's like this</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>doing</t>
+  </si>
+  <si>
+    <t>Make repositories</t>
+  </si>
+  <si>
+    <t>Make controllers</t>
+  </si>
+  <si>
+    <t>Create a user stories</t>
+  </si>
+  <si>
+    <t>Create and enter a user stories in product backlog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User story </t>
+  </si>
+  <si>
+    <t>Start user story(#1) - make crud for planner of the assignments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start planner view for user story(#1) </t>
+  </si>
+  <si>
+    <t>Create project management document structure(PB, sprints, gannt diagramm )</t>
+  </si>
 </sst>
 </file>
 
@@ -861,7 +936,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1020,6 +1095,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1029,7 +1166,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1186,6 +1323,35 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="2" xr:uid="{52E8FA25-AB34-439C-BC48-9650F425CC09}"/>
@@ -1316,6 +1482,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC65911"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="7"/>
       </font>
     </dxf>
@@ -1365,11 +1536,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC65911"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1447,7 +1613,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>deliverable 1</a:t>
+            <a:t>deliverable sprint 1</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1473,7 +1639,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Organize product backlog :</a:t>
+            <a:t>Organize Product Backlog(PB) :</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1487,7 +1653,15 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t> -  PL item prioritization</a:t>
+            <a:t> -  PB</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>item prioritization</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1679,7 +1853,107 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+            <a:buChar char="Ø"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Structure</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="171450" indent="-171450">
+            <a:buFont typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+            <a:buChar char="Ø"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Description of code in parallel with a code state.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7767639" cy="971550"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F701DBF-173C-4E33-801B-433AE780A996}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3714750"/>
+          <a:ext cx="7767639" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>The main aspects of Sprint 1 were:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>1.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> Creation of project management.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>2. Working with user story #1.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t>3. Creating of ducument structure.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2446,7 +2720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13538CB-7E67-4044-B4BC-9356A4A96686}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2468,24 +2742,24 @@
     </row>
     <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="72" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H2" s="77" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F3" s="74" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H3" s="77" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -2493,23 +2767,23 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H5" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" t="s">
         <v>87</v>
-      </c>
-      <c r="I5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H6" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
         <v>88</v>
-      </c>
-      <c r="I6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="57" x14ac:dyDescent="0.45">
@@ -2521,13 +2795,13 @@
         <v>44217</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H7" s="79">
         <v>16</v>
       </c>
       <c r="I7" s="49" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
@@ -2542,13 +2816,13 @@
         <v>44218</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H9" s="79" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
@@ -2560,13 +2834,13 @@
         <v>44218</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H10" s="68" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
@@ -2578,69 +2852,69 @@
         <v>44217</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H11" s="79" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F12" s="74" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H12" s="68" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F16" s="81" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="6:10" x14ac:dyDescent="0.45">
       <c r="I17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="6:10" x14ac:dyDescent="0.45">
       <c r="I18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="6:10" x14ac:dyDescent="0.45">
       <c r="F19" s="74" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="6:10" x14ac:dyDescent="0.45">
       <c r="J20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="6:10" x14ac:dyDescent="0.45">
       <c r="I21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J21" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2667,23 +2941,23 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E4" s="76">
         <f>D4-C4</f>
@@ -2692,11 +2966,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" s="74">
         <f ca="1">TODAY()</f>
-        <v>44091</v>
+        <v>44103</v>
       </c>
       <c r="C5" s="75">
         <v>0.65625</v>
@@ -2962,8 +3236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB44EE33-8DB4-4D77-8C2D-5A0F5796B97D}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3005,7 +3279,7 @@
         <v>21</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -3209,8 +3483,8 @@
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" s="21">
-        <v>15</v>
+      <c r="A21" s="21" t="s">
+        <v>115</v>
       </c>
       <c r="B21" s="16">
         <v>44200</v>
@@ -3282,8 +3556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ER23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3314,7 +3588,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="64" t="s">
         <v>1</v>
@@ -4092,7 +4366,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="51" t="s">
         <v>5</v>
@@ -4101,13 +4375,13 @@
         <v>26</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="51" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H7" s="60" t="s">
         <v>14</v>
@@ -5269,11 +5543,11 @@
       </c>
       <c r="B9" s="53" t="str">
         <f>'Sprint 1'!B7</f>
-        <v xml:space="preserve">User stories </v>
+        <v>Create a user stories</v>
       </c>
       <c r="C9" s="54" t="str">
         <f>'Sprint 1'!C7</f>
-        <v>Enter user stories in product backlog</v>
+        <v>Create and enter a user stories in product backlog</v>
       </c>
       <c r="D9" s="54" t="str">
         <f>'Sprint 1'!E7</f>
@@ -9400,7 +9674,7 @@
       </c>
       <c r="C16" s="54" t="str">
         <f>'Sprint 1'!C14</f>
-        <v xml:space="preserve">Start first steps of study director's view design with Blazor </v>
+        <v xml:space="preserve">Start planner view for user story(#1) </v>
       </c>
       <c r="D16" s="54" t="str">
         <f>'Sprint 1'!E14</f>
@@ -12783,35 +13057,35 @@
     <row r="23" spans="1:148" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="I24:EP1048576 AD23:EP23 J18:EP22 I6:EP6 I5:ER5 I7:ER17 I3:EP4 I2:AD2 AH2:EP2">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:EH22 I8:ER17">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>High</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D13">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:EN6">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"m"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D17">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12822,35 +13096,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7E729C-7B33-4373-8A6D-2CA0A89FC9F4}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.53125" customWidth="1"/>
     <col min="2" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="3" width="104.73046875" customWidth="1"/>
+    <col min="3" max="3" width="78.265625" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="6.86328125" customWidth="1"/>
     <col min="7" max="7" width="6.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="str">
         <f>Gannt!A1</f>
         <v>BaThesis BTI7321 20/21, HS, Project Planning</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="70" t="s">
         <v>23</v>
       </c>
@@ -12872,104 +13146,158 @@
       <c r="G4" s="70" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H4" s="82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="69">
         <v>1</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="C5" s="71" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="D5" s="69" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G5" s="69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="69">
         <v>2</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
+        <v>70</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E6" s="69"/>
       <c r="F6" s="69"/>
       <c r="G6" s="69"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="69">
         <v>3</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
+      <c r="B7" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E7" s="69"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="69">
         <v>4</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
+      <c r="B8" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E8" s="69"/>
       <c r="F8" s="69"/>
       <c r="G8" s="69"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="69">
         <v>5</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
+      <c r="B9" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="69"/>
       <c r="F9" s="69"/>
       <c r="G9" s="69"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="69">
         <v>6</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
+      <c r="B10" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E10" s="69"/>
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="69">
         <v>7</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
+      <c r="B11" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>38</v>
+      </c>
       <c r="E11" s="69"/>
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="69">
         <v>8</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
+      <c r="B12" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>135</v>
+      </c>
       <c r="E12" s="69"/>
       <c r="F12" s="69"/>
       <c r="G12" s="69"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="69">
         <v>9</v>
       </c>
@@ -12980,7 +13308,7 @@
       <c r="F13" s="69"/>
       <c r="G13" s="69"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="69">
         <v>10</v>
       </c>
@@ -12991,7 +13319,7 @@
       <c r="F14" s="69"/>
       <c r="G14" s="69"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="69">
         <v>11</v>
       </c>
@@ -13002,7 +13330,7 @@
       <c r="F15" s="69"/>
       <c r="G15" s="69"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="69">
         <v>12</v>
       </c>
@@ -13179,7 +13507,350 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.796875" customWidth="1"/>
+    <col min="2" max="2" width="19.3984375" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="9.06640625" style="42"/>
+    <col min="8" max="8" width="7.796875" customWidth="1"/>
+    <col min="9" max="9" width="8.9296875" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" t="str">
+        <f>Gannt!A1</f>
+        <v>BaThesis BTI7321 20/21, HS, Project Planning</v>
+      </c>
+      <c r="I1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
+      <c r="A2" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F3">
+        <f>SUM(F5:F15)</f>
+        <v>91</v>
+      </c>
+      <c r="G3" s="13">
+        <f>SUM(G5:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="88">
+        <v>1</v>
+      </c>
+      <c r="B5" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="90">
+        <f>F5/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="14">
+        <v>2</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="92"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="88">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="89" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="90">
+        <f>F6/4</f>
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="14">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="92"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="88">
+        <v>2</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="90">
+        <f t="shared" ref="D7:D15" si="0">F7/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="14">
+        <v>2</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="92"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="88">
+        <v>3</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="90">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="92"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="88">
+        <v>5</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="90">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="92"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="88">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="90">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="14">
+        <v>20</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="92"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="88">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="90">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="14">
+        <v>10</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="92"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="88">
+        <v>4</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="90">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="14">
+        <v>10</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="92"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="88">
+        <v>7</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="90">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="14">
+        <v>10</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="92"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="88">
+        <v>9</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="90">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="E14" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="14">
+        <v>5</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="92"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="93">
+        <v>10</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="94">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0</v>
+      </c>
+      <c r="G15" s="29"/>
+      <c r="H15" s="96"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="E5:E22" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I18">
+      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="14"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="E4:E15">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8346C48C-640E-494D-85F6-A16EC8AEE9A1}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13201,302 +13872,10 @@
     </row>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="F3">
-        <f>SUM(F5:F15)</f>
-        <v>91</v>
-      </c>
-      <c r="G3" s="13">
-        <f>SUM(G5:G15)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="44">
-        <f>F5/4</f>
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="44">
-        <f>F6/4</f>
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="44">
-        <f t="shared" ref="D7:D15" si="0">F7/4</f>
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="44">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="D9" s="44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="D10" s="44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="D11" s="44">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="D12" s="44">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="D13" s="44">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="44">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="E5:E22" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:I18">
-      <sortCondition sortBy="fontColor" ref="E5:E18" dxfId="21"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="E4:E15">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>"High"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8346C48C-640E-494D-85F6-A16EC8AEE9A1}">
-  <dimension ref="A1:I12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="15.59765625" customWidth="1"/>
-    <col min="3" max="3" width="30.59765625" customWidth="1"/>
-    <col min="4" max="4" width="13.73046875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="9.06640625" style="42"/>
-    <col min="8" max="8" width="7.796875" customWidth="1"/>
-    <col min="9" max="9" width="17.796875" customWidth="1"/>
-    <col min="10" max="10" width="40" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" t="str">
-        <f>Gannt!A1</f>
-        <v>BaThesis BTI7321 20/21, HS, Project Planning</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="A2" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -13509,7 +13888,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -13523,7 +13902,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>26</v>
@@ -13543,47 +13922,47 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -13638,7 +14017,7 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -13651,7 +14030,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -13665,7 +14044,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>26</v>
@@ -13710,7 +14089,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13735,7 +14114,7 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -13748,7 +14127,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -13762,7 +14141,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>26</v>
@@ -13832,7 +14211,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -13841,10 +14220,10 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -13883,7 +14262,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -13914,7 +14293,7 @@
         <v>M</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -13945,7 +14324,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -13987,7 +14366,7 @@
     </row>
     <row r="11" spans="1:21" ht="171" x14ac:dyDescent="0.45">
       <c r="A11" s="73" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>

</xml_diff>

<commit_message>
some changes in epic table
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7165AE-D811-4A93-9D1A-A96A21BDD778}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604F8397-C567-4861-AFAB-5153661C4E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1163" yWindow="1222" windowWidth="10800" windowHeight="5461" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="165">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -820,7 +820,14 @@
     </r>
   </si>
   <si>
-    <t>Display module run in concrete semester</t>
+    <t>Display module run for one concrete semester</t>
+  </si>
+  <si>
+    <t>Build new entities in backend, 
+connect it to the whole programm</t>
+  </si>
+  <si>
+    <t>Testing with postman</t>
   </si>
 </sst>
 </file>
@@ -1431,7 +1438,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1669,6 +1676,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="2" xr:uid="{52E8FA25-AB34-439C-BC48-9650F425CC09}"/>
@@ -1676,7 +1686,7 @@
     <cellStyle name="Title" xfId="3" builtinId="15"/>
     <cellStyle name="zHiddenText" xfId="1" xr:uid="{5343EAB6-CD30-48D5-9BB1-01A341256D68}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="19">
     <dxf>
       <font>
         <color theme="8" tint="0.79998168889431442"/>
@@ -1769,37 +1779,7 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
+        <color rgb="FFC65911"/>
       </font>
     </dxf>
     <dxf>
@@ -1853,11 +1833,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC65911"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2510,7 +2485,6 @@
             <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>code:</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr marL="171450" indent="-171450">
@@ -2519,7 +2493,7 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Controllers</a:t>
+            <a:t>New enities </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3371,7 +3345,7 @@
       </c>
       <c r="B5" s="66">
         <f ca="1">TODAY()</f>
-        <v>44116</v>
+        <v>44128</v>
       </c>
       <c r="C5" s="67">
         <v>0.65625</v>
@@ -13998,35 +13972,35 @@
     <row r="24" spans="1:149" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="J25:EQ1048576 AE24:EQ24 K22:EQ23 J6:EQ6 J5:ES5 J7:ES8 J3:EQ4 J2:AE2 AI2:EQ2 EJ9:ES18 EJ19:EQ21 J9:EI21">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:EI23 EJ9:ES18 J9:EI21">
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>High</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:EO6">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"m"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14947,11 +14921,11 @@
   </sheetData>
   <autoFilter ref="F5:F24" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J20">
-      <sortCondition sortBy="fontColor" ref="F5:F20" dxfId="22"/>
+      <sortCondition sortBy="fontColor" ref="F5:F20" dxfId="11"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F4:F17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14965,7 +14939,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -15016,7 +14990,7 @@
       </c>
       <c r="G3">
         <f>SUM(G6:G18)</f>
-        <v>34.5</v>
+        <v>46</v>
       </c>
       <c r="H3" s="13">
         <f>SUM(H6:H18)</f>
@@ -15216,22 +15190,28 @@
       <c r="H10" s="82"/>
       <c r="I10" s="83"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="126">
         <v>20</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="C11" s="129" t="s">
+        <v>163</v>
+      </c>
       <c r="D11" s="98">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9444444444444442</v>
       </c>
       <c r="E11" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
-      </c>
-      <c r="F11" s="82"/>
-      <c r="G11" s="82"/>
+        <v>8.6527777777777768</v>
+      </c>
+      <c r="F11" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="82">
+        <v>10</v>
+      </c>
       <c r="H11" s="82"/>
       <c r="I11" s="83"/>
     </row>
@@ -15240,17 +15220,23 @@
         <v>21</v>
       </c>
       <c r="B12" s="14"/>
-      <c r="C12" s="87"/>
+      <c r="C12" s="87" t="s">
+        <v>164</v>
+      </c>
       <c r="D12" s="98">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="E12" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
-      </c>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
+        <v>8.9444444444444429</v>
+      </c>
+      <c r="F12" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="82">
+        <v>1.5</v>
+      </c>
       <c r="H12" s="119"/>
       <c r="I12" s="83"/>
     </row>
@@ -15264,7 +15250,7 @@
       </c>
       <c r="E13" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F13" s="82"/>
       <c r="G13" s="119"/>
@@ -15281,7 +15267,7 @@
       </c>
       <c r="E14" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F14" s="82"/>
       <c r="G14" s="119"/>
@@ -15298,7 +15284,7 @@
       </c>
       <c r="E15" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F15" s="82"/>
       <c r="G15" s="119"/>
@@ -15315,7 +15301,7 @@
       </c>
       <c r="E16" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F16" s="82"/>
       <c r="G16" s="119"/>
@@ -15332,7 +15318,7 @@
       </c>
       <c r="E17" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F17" s="82"/>
       <c r="G17" s="119"/>
@@ -15340,9 +15326,7 @@
       <c r="I17" s="83"/>
     </row>
     <row r="18" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="80">
-        <v>13</v>
-      </c>
+      <c r="A18" s="80"/>
       <c r="B18" s="29" t="s">
         <v>37</v>
       </c>
@@ -15355,7 +15339,7 @@
       </c>
       <c r="E18" s="98">
         <f t="shared" si="1"/>
-        <v>6.7083333333333321</v>
+        <v>8.9444444444444429</v>
       </c>
       <c r="F18" s="84" t="s">
         <v>37</v>
@@ -15368,7 +15352,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F4:F18">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added update semester method in semester controller
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1500F4-6DDF-482F-8FF7-3F77A137C815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E441D7-134B-46B0-9A8C-4E28C9346BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="185">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -891,8 +891,8 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yy"/>
     <numFmt numFmtId="165" formatCode="dd"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="168" formatCode="ddd"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="ddd"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -1711,7 +1711,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1746,14 +1746,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1773,7 +1773,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1791,8 +1791,8 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1804,7 +1804,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1878,7 +1878,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1886,8 +1886,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1952,6 +1952,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC65911"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="7"/>
       </font>
     </dxf>
@@ -2001,11 +2006,6 @@
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC65911"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2125,6 +2125,12 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>4. Poster</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>5. Video</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -3490,10 +3496,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3759,7 +3761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13538CB-7E67-4044-B4BC-9356A4A96686}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4110,7 +4112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB44EE33-8DB4-4D77-8C2D-5A0F5796B97D}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -14478,35 +14480,35 @@
     <row r="24" spans="1:149" ht="21.4" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <conditionalFormatting sqref="J25:EQ1048576 AE24:EQ24 K22:EQ23 J6:EQ6 J5:ES5 J7:ES8 J3:EQ4 J2:AE2 AI2:EQ2 EJ9:ES18 EJ19:EQ21 J9:EI21">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:EI23 EJ9:ES18 J9:EI21">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>High</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:EO6">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"m"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D21">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14527,7 +14529,7 @@
   <cols>
     <col min="1" max="1" width="2.53125" customWidth="1"/>
     <col min="2" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="3" width="78.265625" customWidth="1"/>
+    <col min="3" max="3" width="70.86328125" customWidth="1"/>
     <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="6.86328125" customWidth="1"/>
@@ -15459,7 +15461,7 @@
   </sheetData>
   <autoFilter ref="F5:F25" xr:uid="{19388B08-6607-4FB7-80A4-7440077A6089}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J21">
-      <sortCondition sortBy="fontColor" ref="F5:F21" dxfId="13"/>
+      <sortCondition sortBy="fontColor" ref="F5:F21" dxfId="6"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="F4:F18">
@@ -16010,8 +16012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16156,7 +16158,9 @@
         <v>1.5</v>
       </c>
       <c r="H6" s="69"/>
-      <c r="I6" s="70"/>
+      <c r="I6" s="70" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="111">
@@ -16210,7 +16214,9 @@
         <v>12</v>
       </c>
       <c r="H8" s="69"/>
-      <c r="I8" s="70"/>
+      <c r="I8" s="70" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="111">
@@ -16227,7 +16233,7 @@
         <v>0.9722222222222221</v>
       </c>
       <c r="E9" s="83">
-        <f t="shared" ref="E9:E19" si="1">D9+E8</f>
+        <f t="shared" ref="E9:E18" si="1">D9+E8</f>
         <v>5.1527777777777777</v>
       </c>
       <c r="F9" s="69" t="s">

</xml_diff>

<commit_message>
semester can be updated in the view
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E441D7-134B-46B0-9A8C-4E28C9346BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2867CAB-6E39-402A-B09B-AF41B7FC3700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="185">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -15478,8 +15478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8346C48C-640E-494D-85F6-A16EC8AEE9A1}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16012,8 +16012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16243,7 +16243,9 @@
         <v>5</v>
       </c>
       <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
+      <c r="I9" s="70" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="112">
@@ -16375,7 +16377,9 @@
         <v>8</v>
       </c>
       <c r="H14" s="104"/>
-      <c r="I14" s="70"/>
+      <c r="I14" s="70" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="111">
@@ -16899,7 +16903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91297CB-FE51-46A7-A70E-391CFFF80B75}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added UI Specification in report
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2867CAB-6E39-402A-B09B-AF41B7FC3700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7793C86-5A71-492E-BA4E-9E22A89FB680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="185">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -4112,7 +4112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB44EE33-8DB4-4D77-8C2D-5A0F5796B97D}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -16012,8 +16012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16072,7 +16072,7 @@
       </c>
       <c r="H3" s="13">
         <f>SUM(H6:H19)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J3" t="s">
         <v>117</v>
@@ -16129,8 +16129,12 @@
       <c r="G5" s="113">
         <v>1</v>
       </c>
-      <c r="H5" s="105"/>
-      <c r="I5" s="108"/>
+      <c r="H5" s="105">
+        <v>1</v>
+      </c>
+      <c r="I5" s="108" t="s">
+        <v>107</v>
+      </c>
       <c r="J5" s="109"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
@@ -16157,7 +16161,9 @@
       <c r="G6" s="69">
         <v>1.5</v>
       </c>
-      <c r="H6" s="69"/>
+      <c r="H6" s="69">
+        <v>1.5</v>
+      </c>
       <c r="I6" s="70" t="s">
         <v>107</v>
       </c>
@@ -16187,7 +16193,9 @@
         <v>8</v>
       </c>
       <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
+      <c r="I7" s="70" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="112">
@@ -16903,7 +16911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91297CB-FE51-46A7-A70E-391CFFF80B75}">
   <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new domain model, changed UI requirements
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7793C86-5A71-492E-BA4E-9E22A89FB680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA3953-BE55-4F9D-A2F1-CFB73C49E29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -1604,7 +1604,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1906,6 +1906,10 @@
     </xf>
     <xf numFmtId="16" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3420,6 +3424,230 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57152</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4567236" cy="1895475"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E5710B-8B8F-492E-9579-677F0805D27E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4505327" y="4443413"/>
+          <a:ext cx="4567236" cy="1895475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>brake</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1" baseline="0">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> plan into days plan</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" b="1">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>report</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>describe layers and architecture , add</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> layer diagram, finish sith ui requirements and UI in general</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" baseline="0">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>code</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>23-Nov</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>&gt; finish with all repo and make services </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>24,25,26,27-Nov</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>add backend logic into services</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>28,29-Nov</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>write new controllers</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3494,6 +3722,10 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4113,7 +4345,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4355,7 +4587,7 @@
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="73">
-        <v>44185</v>
+        <v>44194</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -16010,10 +16242,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16072,7 +16304,7 @@
       </c>
       <c r="H3" s="13">
         <f>SUM(H6:H19)</f>
-        <v>1.5</v>
+        <v>10.5</v>
       </c>
       <c r="J3" t="s">
         <v>117</v>
@@ -16192,7 +16424,9 @@
       <c r="G7" s="69">
         <v>8</v>
       </c>
-      <c r="H7" s="69"/>
+      <c r="H7" s="69">
+        <v>9</v>
+      </c>
       <c r="I7" s="70" t="s">
         <v>98</v>
       </c>
@@ -16484,6 +16718,13 @@
       </c>
       <c r="H19" s="71"/>
       <c r="I19" s="72"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B22" s="15"/>
+      <c r="D22" s="161"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B23" s="160"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F4:F9 F11:F19">

</xml_diff>

<commit_message>
added plan service and controller
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA3953-BE55-4F9D-A2F1-CFB73C49E29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF473203-0597-4E5A-8926-41592200A382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="190">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -881,6 +881,21 @@
       </rPr>
       <t>zwischen 25.1. und</t>
     </r>
+  </si>
+  <si>
+    <t>till 7Jan2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">book </t>
+  </si>
+  <si>
+    <t>book ---&gt; Mr.Pfahrer</t>
+  </si>
+  <si>
+    <t>book----------&gt; Mr. Pfahrer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> delivery of sprint3</t>
   </si>
 </sst>
 </file>
@@ -3724,10 +3739,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3993,8 +4004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13538CB-7E67-4044-B4BC-9356A4A96686}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4323,10 +4334,16 @@
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="14"/>
       <c r="B20" s="150"/>
-      <c r="C20" s="131"/>
+      <c r="C20" s="131" t="s">
+        <v>185</v>
+      </c>
       <c r="D20" s="136"/>
-      <c r="E20" s="142"/>
-      <c r="F20" s="156"/>
+      <c r="E20" s="142" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" s="156" t="s">
+        <v>187</v>
+      </c>
       <c r="G20" s="126"/>
       <c r="H20" s="126"/>
       <c r="I20" s="126"/>
@@ -4345,7 +4362,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4560,7 +4577,7 @@
       <c r="D16" s="34"/>
       <c r="E16" s="59"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="21">
         <v>13</v>
       </c>
@@ -4575,7 +4592,7 @@
       </c>
       <c r="E17" s="59"/>
     </row>
-    <row r="18" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="23">
         <v>14</v>
       </c>
@@ -4590,7 +4607,7 @@
         <v>44194</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="25" t="s">
         <v>18</v>
       </c>
@@ -4602,7 +4619,7 @@
       </c>
       <c r="D19" s="28"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
         <v>18</v>
       </c>
@@ -4614,7 +4631,7 @@
       </c>
       <c r="D20" s="157"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="21" t="s">
         <v>80</v>
       </c>
@@ -4625,8 +4642,14 @@
         <v>44204</v>
       </c>
       <c r="D21" s="157"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E21" s="160">
+        <v>43837</v>
+      </c>
+      <c r="F21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="21">
         <v>16</v>
       </c>
@@ -4643,7 +4666,7 @@
         <v>43851</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="14"/>
       <c r="B23" s="16">
         <v>44214</v>
@@ -4653,7 +4676,7 @@
       </c>
       <c r="D23" s="157"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="14"/>
       <c r="B24" s="16">
         <v>44221</v>
@@ -4663,7 +4686,7 @@
       </c>
       <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="14"/>
       <c r="B25" s="16">
         <v>44228</v>
@@ -4673,7 +4696,7 @@
       </c>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="29"/>
       <c r="B26" s="24">
         <v>44235</v>
@@ -16244,8 +16267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16703,7 +16726,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>133</v>
+        <v>189</v>
       </c>
       <c r="D19" s="83">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
added navigation bar view
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF473203-0597-4E5A-8926-41592200A382}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88966EE8-D4B9-4398-B81F-49D48AE0A245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3655,6 +3655,20 @@
             <a:rPr lang="en-US"/>
             <a:t> </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>28,29 - implement</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" baseline="0">
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> UIs</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
           </a:endParaRPr>
@@ -16267,7 +16281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added service for planlecturer in web project
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01A693D-A2EA-4F03-9DD5-CB8ECBD0B24F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AF16C7-E295-4C49-8852-9DFE9601D6FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="207">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -4836,7 +4836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB44EE33-8DB4-4D77-8C2D-5A0F5796B97D}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -17298,8 +17298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2687EE61-BC21-474A-A1F5-FD35F1C9EE1C}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17357,7 +17357,7 @@
       </c>
       <c r="H3" s="13">
         <f>SUM(H6:H19)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="J3" t="s">
         <v>117</v>
@@ -17442,8 +17442,12 @@
       <c r="G6" s="63">
         <v>1.5</v>
       </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="H6" s="63">
+        <v>1.5</v>
+      </c>
+      <c r="I6" s="64" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="105">
@@ -17526,7 +17530,7 @@
       <c r="H9" s="63"/>
       <c r="I9" s="64"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="13.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="106">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
added more information to the management chapter of report
</commit_message>
<xml_diff>
--- a/3project_management/project_management.xlsx
+++ b/3project_management/project_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PLANA\planning-of-the-assignments-for-lecturers-plana\3project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A72C9F-3A1D-45A6-9688-6030F816D5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120BC33A-8479-4F6C-8102-1C4ECA7181A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Termins-rules" sheetId="9" r:id="rId1"/>
@@ -790,9 +790,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="167" formatCode="ddd"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="165" formatCode="ddd"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1246,8 +1246,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1259,7 +1259,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFill="1"/>
@@ -1279,8 +1279,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1302,10 +1302,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1314,14 +1314,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,7 +1335,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1346,7 +1346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1355,19 +1355,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1404,16 +1404,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1441,22 +1441,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1875,16 +1875,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr marL="171450" indent="-171450">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>   - schedule the tasks using gannt diagram</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
           <a:pPr marL="0" indent="0">
             <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             <a:buNone/>
@@ -2281,16 +2271,6 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>   - schedule the tasks using gannt diagram</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buNone/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
             <a:t>  </a:t>
           </a:r>
         </a:p>
@@ -2813,7 +2793,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>   - schedule the tasks using gannt diagram</a:t>
+            <a:t>   </a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -4623,7 +4603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D544E4EA-43A9-4C2D-95F8-E8BC054D1071}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -5676,7 +5656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6800609C-959E-46C1-840F-B86053269743}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5905,7 +5885,7 @@
         <v>124</v>
       </c>
       <c r="D9" s="46">
-        <f t="shared" ref="D9:D19" si="0">G9/F$3</f>
+        <f t="shared" ref="D9:D18" si="0">G9/F$3</f>
         <v>0.9722222222222221</v>
       </c>
       <c r="E9" s="46">
@@ -6466,11 +6446,11 @@
         <v>152</v>
       </c>
       <c r="D9" s="46">
-        <f t="shared" ref="D9:D19" si="0">G9/F$3</f>
+        <f t="shared" ref="D9:D18" si="0">G9/F$3</f>
         <v>2.9166666666666665</v>
       </c>
       <c r="E9" s="46">
-        <f t="shared" ref="E9:E19" si="1">D9+E8</f>
+        <f t="shared" ref="E9:E18" si="1">D9+E8</f>
         <v>16.819444444444443</v>
       </c>
       <c r="F9" s="32" t="s">

</xml_diff>